<commit_message>
Update HW air quality v2 + update BOMs
</commit_message>
<xml_diff>
--- a/hardware/Buttons/bom/Buttons.xlsx
+++ b/hardware/Buttons/bom/Buttons.xlsx
@@ -1,6 +1,6 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" mc:Ignorable="x15 xr xr6 xr10">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23929"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
@@ -8,19 +8,30 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\JonaCappelle\Documents\Github\sensors\hardware\Buttons\bom\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:40009_{3975CBAF-202D-4415-869B-24586FA9D15C}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A154931E-FFD5-4F7D-8872-14AF36E0BAA3}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15990"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15990" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Buttons" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="0"/>
+  <calcPr calcId="191029"/>
+  <extLst>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+      </xcalcf:calcFeatures>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="40" uniqueCount="35">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="59" uniqueCount="50">
   <si>
     <t>Id</t>
   </si>
@@ -37,9 +48,6 @@
     <t>Orientatie</t>
   </si>
   <si>
-    <t>Leverancier en ref</t>
-  </si>
-  <si>
     <t>REF**</t>
   </si>
   <si>
@@ -125,13 +133,61 @@
   </si>
   <si>
     <t>10k</t>
+  </si>
+  <si>
+    <t>Ordercode Farnell</t>
+  </si>
+  <si>
+    <t>Ordercode Mouser</t>
+  </si>
+  <si>
+    <t>979-3006.2114</t>
+  </si>
+  <si>
+    <t>C0805C104M4RACAUTO</t>
+  </si>
+  <si>
+    <t>Reel</t>
+  </si>
+  <si>
+    <t>MCWR08X1001FTL</t>
+  </si>
+  <si>
+    <t>KP-2012QBC-D</t>
+  </si>
+  <si>
+    <t>MC01W08051100K</t>
+  </si>
+  <si>
+    <t>MC01W0805110K</t>
+  </si>
+  <si>
+    <t>PIC16F18446-I/SS</t>
+  </si>
+  <si>
+    <t>Type</t>
+  </si>
+  <si>
+    <t>Not specified</t>
+  </si>
+  <si>
+    <t>Manufacturer Part Number (MPN)</t>
+  </si>
+  <si>
+    <t>Tape en reel, afgesneden</t>
+  </si>
+  <si>
+    <t>M20-9980345</t>
+  </si>
+  <si>
+    <t>Per stuk</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="18" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <fonts count="20" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -265,6 +321,18 @@
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="8"/>
+      <color rgb="FF333333"/>
+      <name val="Verdana"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color rgb="FF333333"/>
+      <name val="Arial"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="35">
@@ -620,11 +688,23 @@
     <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="33" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="34" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="3" fontId="0" fillId="34" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="3" fontId="19" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="42">
     <cellStyle name="20% - Accent1" xfId="19" builtinId="30" customBuiltin="1"/>
@@ -979,21 +1059,25 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F13"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:I13"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F19" sqref="F19"/>
+      <selection activeCell="F3" sqref="F3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="2" max="2" width="18.7109375" customWidth="1"/>
     <col min="3" max="3" width="39.85546875" customWidth="1"/>
-    <col min="5" max="5" width="27.7109375" customWidth="1"/>
+    <col min="5" max="5" width="36.85546875" customWidth="1"/>
+    <col min="6" max="6" width="24.42578125" style="5" customWidth="1"/>
+    <col min="7" max="7" width="21.7109375" style="5" customWidth="1"/>
+    <col min="8" max="8" width="23.28515625" style="5" customWidth="1"/>
+    <col min="9" max="9" width="28.42578125" style="5" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -1009,67 +1093,76 @@
       <c r="E1" t="s">
         <v>4</v>
       </c>
-      <c r="F1" t="s">
+      <c r="F1" s="5" t="s">
+        <v>46</v>
+      </c>
+      <c r="G1" s="5" t="s">
+        <v>34</v>
+      </c>
+      <c r="H1" s="5" t="s">
+        <v>35</v>
+      </c>
+      <c r="I1" s="5" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A2" s="1">
+        <v>1</v>
+      </c>
+      <c r="B2" s="1" t="s">
         <v>5</v>
       </c>
+      <c r="C2" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="D2" s="1">
+        <v>1</v>
+      </c>
+      <c r="E2" s="1" t="s">
+        <v>6</v>
+      </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A2" s="2">
-        <v>1</v>
-      </c>
-      <c r="B2" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="C2" s="2" t="s">
-        <v>7</v>
-      </c>
-      <c r="D2" s="2">
-        <v>1</v>
-      </c>
-      <c r="E2" s="2" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A3" s="1">
         <v>2</v>
       </c>
       <c r="B3" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="C3" s="1" t="s">
         <v>8</v>
-      </c>
-      <c r="C3" s="1" t="s">
-        <v>9</v>
       </c>
       <c r="D3" s="1">
         <v>1</v>
       </c>
       <c r="E3" s="1" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A4" s="1">
         <v>3</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="D4" s="1">
         <v>1</v>
       </c>
       <c r="E4" s="1" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
     </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A5" s="2">
         <v>4</v>
       </c>
       <c r="B5" s="2" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="C5" s="2">
         <v>30062114</v>
@@ -1080,144 +1173,217 @@
       <c r="E5" s="3">
         <v>30062114</v>
       </c>
+      <c r="F5" s="6">
+        <v>30062114</v>
+      </c>
+      <c r="H5" s="7" t="s">
+        <v>36</v>
+      </c>
+      <c r="I5" s="5" t="s">
+        <v>45</v>
+      </c>
     </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A6" s="2">
         <v>5</v>
       </c>
       <c r="B6" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="C6" s="2" t="s">
         <v>13</v>
-      </c>
-      <c r="C6" s="2" t="s">
-        <v>14</v>
       </c>
       <c r="D6" s="2">
         <v>1</v>
       </c>
       <c r="E6" s="2" t="s">
-        <v>15</v>
+        <v>14</v>
+      </c>
+      <c r="F6" s="4" t="s">
+        <v>48</v>
+      </c>
+      <c r="G6" s="4">
+        <v>1022230</v>
+      </c>
+      <c r="I6" s="5" t="s">
+        <v>49</v>
       </c>
     </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A7" s="2">
         <v>6</v>
       </c>
       <c r="B7" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="C7" s="2" t="s">
         <v>16</v>
-      </c>
-      <c r="C7" s="2" t="s">
-        <v>17</v>
       </c>
       <c r="D7" s="2">
         <v>5</v>
       </c>
       <c r="E7" s="2" t="s">
-        <v>18</v>
+        <v>17</v>
+      </c>
+      <c r="F7" s="4" t="s">
+        <v>37</v>
+      </c>
+      <c r="G7" s="4">
+        <v>3510057</v>
+      </c>
+      <c r="I7" s="5" t="s">
+        <v>38</v>
       </c>
     </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A8" s="2">
         <v>7</v>
       </c>
       <c r="B8" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="C8" s="2" t="s">
         <v>19</v>
-      </c>
-      <c r="C8" s="2" t="s">
-        <v>20</v>
       </c>
       <c r="D8" s="2">
         <v>5</v>
       </c>
       <c r="E8" s="2" t="s">
-        <v>21</v>
+        <v>20</v>
+      </c>
+      <c r="F8" s="4" t="s">
+        <v>39</v>
+      </c>
+      <c r="G8" s="4">
+        <v>2446904</v>
+      </c>
+      <c r="I8" s="5" t="s">
+        <v>38</v>
       </c>
     </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A9" s="2">
         <v>8</v>
       </c>
       <c r="B9" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="C9" s="2" t="s">
         <v>22</v>
-      </c>
-      <c r="C9" s="2" t="s">
-        <v>23</v>
       </c>
       <c r="D9" s="2">
         <v>1</v>
       </c>
       <c r="E9" s="2" t="s">
-        <v>24</v>
+        <v>23</v>
+      </c>
+      <c r="F9" s="4" t="s">
+        <v>40</v>
+      </c>
+      <c r="G9" s="4">
+        <v>2217974</v>
+      </c>
+      <c r="I9" s="5" t="s">
+        <v>47</v>
       </c>
     </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A10" s="2">
         <v>9</v>
       </c>
       <c r="B10" s="2" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="C10" s="2" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="D10" s="2">
         <v>4</v>
       </c>
       <c r="E10" s="2" t="s">
-        <v>26</v>
+        <v>25</v>
+      </c>
+      <c r="F10" s="4" t="s">
+        <v>41</v>
+      </c>
+      <c r="G10" s="4">
+        <v>2129276</v>
+      </c>
+      <c r="I10" s="5" t="s">
+        <v>38</v>
       </c>
     </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A11" s="1">
         <v>10</v>
       </c>
       <c r="B11" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="C11" s="1" t="s">
         <v>27</v>
-      </c>
-      <c r="C11" s="1" t="s">
-        <v>28</v>
       </c>
       <c r="D11" s="1">
         <v>1</v>
       </c>
       <c r="E11" s="1" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
     </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A12" s="2">
         <v>11</v>
       </c>
       <c r="B12" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="C12" s="2" t="s">
         <v>30</v>
-      </c>
-      <c r="C12" s="2" t="s">
-        <v>31</v>
       </c>
       <c r="D12" s="2">
         <v>1</v>
       </c>
       <c r="E12" s="2" t="s">
-        <v>32</v>
+        <v>31</v>
+      </c>
+      <c r="F12" s="4" t="s">
+        <v>43</v>
+      </c>
+      <c r="G12" s="4">
+        <v>3631504</v>
+      </c>
+      <c r="I12" s="5" t="s">
+        <v>45</v>
       </c>
     </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A13" s="2">
         <v>12</v>
       </c>
       <c r="B13" s="2" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="C13" s="2" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="D13" s="2">
         <v>1</v>
       </c>
       <c r="E13" s="2" t="s">
-        <v>34</v>
+        <v>33</v>
+      </c>
+      <c r="F13" s="4" t="s">
+        <v>42</v>
+      </c>
+      <c r="G13" s="4">
+        <v>2129195</v>
+      </c>
+      <c r="I13" s="5" t="s">
+        <v>38</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>